<commit_message>
11:59 Grafik updatering o planering
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering_PT02.xlsx
+++ b/Grafik/Planering/Grafikplanering_PT02.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
   <si>
     <t>Vecka:</t>
   </si>
@@ -717,7 +717,7 @@
   <dimension ref="A1:AF38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="F29" sqref="F29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,10 +1734,8 @@
       <c r="C29" s="3"/>
       <c r="D29" s="6"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>

</xml_diff>

<commit_message>
12:23 Cloud o planering
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering_PT02.xlsx
+++ b/Grafik/Planering/Grafikplanering_PT02.xlsx
@@ -717,7 +717,7 @@
   <dimension ref="A1:AF38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:G29"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,11 +1039,11 @@
       <c r="C9" s="3"/>
       <c r="D9" s="6"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="W9" s="3"/>
@@ -1065,9 +1065,9 @@
       <c r="C10" s="3"/>
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="7"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>

</xml_diff>

<commit_message>
13:53 Graph plan. update
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering_PT02.xlsx
+++ b/Grafik/Planering/Grafikplanering_PT02.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>Vecka:</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>50% Färdigt</t>
+  </si>
+  <si>
+    <t>1 Dagar</t>
   </si>
 </sst>
 </file>
@@ -720,7 +723,7 @@
   <dimension ref="A1:AF38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25:S25"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +832,7 @@
         <v>62</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="S2" s="12" t="s">
         <v>2</v>
@@ -1043,9 +1046,9 @@
       <c r="D9" s="6"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1111,9 +1114,9 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
-      <c r="AC11" s="7"/>
+      <c r="AC11" s="2"/>
       <c r="AD11" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
@@ -1127,9 +1130,9 @@
       <c r="D12" s="6"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1288,10 +1291,8 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
@@ -1592,9 +1593,9 @@
       <c r="O25" s="6"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="7"/>
+      <c r="R25" s="2"/>
       <c r="S25" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
@@ -2080,9 +2081,9 @@
       <c r="O37" s="6"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="7"/>
+      <c r="R37" s="2"/>
       <c r="S37" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>

</xml_diff>

<commit_message>
15:33 End of Mon
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering_PT02.xlsx
+++ b/Grafik/Planering/Grafikplanering_PT02.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>Vecka:</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>100% Färdigt</t>
-  </si>
-  <si>
-    <t>50% Färdigt</t>
   </si>
   <si>
     <t>1 Dagar</t>
@@ -723,7 +720,7 @@
   <dimension ref="A1:AF38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +829,7 @@
         <v>62</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S2" s="12" t="s">
         <v>2</v>
@@ -1100,9 +1097,9 @@
       <c r="D11" s="6"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1223,9 +1220,9 @@
       <c r="D14" s="6"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1265,11 +1262,11 @@
       <c r="D15" s="6"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="L15" s="10"/>
       <c r="M15" s="11" t="s">
@@ -1305,11 +1302,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="L16" s="10"/>
       <c r="M16" s="11" t="s">
@@ -1629,9 +1626,9 @@
       <c r="O26" s="6"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="7"/>
+      <c r="R26" s="2"/>
       <c r="S26" s="9" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -1793,11 +1790,11 @@
       <c r="O30" s="6"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="R30" s="7"/>
+      <c r="S30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="W30" s="3" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
13:48 eBot - not done
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering_PT02.xlsx
+++ b/Grafik/Planering/Grafikplanering_PT02.xlsx
@@ -720,7 +720,7 @@
   <dimension ref="A1:AF38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,9 +1791,9 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
-      <c r="S30" s="7"/>
+      <c r="S30" s="2"/>
       <c r="T30" s="9" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="U30" s="1"/>
       <c r="W30" s="3" t="s">

</xml_diff>